<commit_message>
Added mobile code countries table
</commit_message>
<xml_diff>
--- a/public/countrystatecity.xlsx
+++ b/public/countrystatecity.xlsx
@@ -1,26 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\Gulf Mall\gulfmall_CMS\src\assets\files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\Gulf Mall\gulfmall_CMS\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A8235A29-A052-4535-9D30-C5FEC044D20A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{D0615681-32D1-4662-907A-88AB446DEBAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
         <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
@@ -31,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>India</t>
   </si>
@@ -67,12 +69,18 @@
   </si>
   <si>
     <t>Country(ar)</t>
+  </si>
+  <si>
+    <t>MobileCode(en)</t>
+  </si>
+  <si>
+    <t>MobileCode(ar)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -416,60 +424,74 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="17.21875" customWidth="1"/>
-    <col min="2" max="2" width="16.44140625" customWidth="1"/>
-    <col min="3" max="3" width="24.44140625" customWidth="1"/>
-    <col min="4" max="4" width="13.88671875" customWidth="1"/>
-    <col min="5" max="5" width="11.44140625" customWidth="1"/>
-    <col min="6" max="6" width="12" customWidth="1"/>
+    <col min="1" max="1" width="16.7265625" customWidth="1"/>
+    <col min="2" max="2" width="15" customWidth="1"/>
+    <col min="3" max="3" width="16.453125" customWidth="1"/>
+    <col min="4" max="4" width="20.08984375" customWidth="1"/>
+    <col min="5" max="5" width="16.453125" customWidth="1"/>
+    <col min="6" max="6" width="15.6328125" customWidth="1"/>
+    <col min="7" max="7" width="13.08984375" customWidth="1"/>
+    <col min="8" max="8" width="13.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2">
+        <v>91</v>
+      </c>
+      <c r="C2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>2</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>3</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2">
+        <v>91</v>
+      </c>
+      <c r="G2" t="s">
         <v>4</v>
       </c>
-      <c r="F2" t="s">
+      <c r="H2" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updated country state city bulf upload template
</commit_message>
<xml_diff>
--- a/public/countrystatecity.xlsx
+++ b/public/countrystatecity.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\Gulf Mall\gulfmall_CMS\public\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\Stalvin_MM\GulfMall\gulfmall_CMS\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D0615681-32D1-4662-907A-88AB446DEBAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A68CE04E-F6BB-4D75-BF96-755C414CE1AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,15 +35,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
-    <t>India</t>
-  </si>
-  <si>
-    <t>Karnataka</t>
-  </si>
-  <si>
-    <t>Bengaluru</t>
-  </si>
-  <si>
     <t>الهند</t>
   </si>
   <si>
@@ -75,13 +66,25 @@
   </si>
   <si>
     <t>MobileCode(ar)</t>
+  </si>
+  <si>
+    <t>Qatar</t>
+  </si>
+  <si>
+    <t>Doha</t>
+  </si>
+  <si>
+    <t>United Arab Emirates</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="\+0"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -96,6 +99,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="7"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Courier New"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -118,9 +127,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -425,74 +437,76 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="16.7265625" customWidth="1"/>
-    <col min="2" max="2" width="15" customWidth="1"/>
+    <col min="2" max="2" width="15" style="4" customWidth="1"/>
     <col min="3" max="3" width="16.453125" customWidth="1"/>
     <col min="4" max="4" width="20.08984375" customWidth="1"/>
     <col min="5" max="5" width="16.453125" customWidth="1"/>
-    <col min="6" max="6" width="15.6328125" customWidth="1"/>
+    <col min="6" max="6" width="15.6328125" style="4" customWidth="1"/>
     <col min="7" max="7" width="13.08984375" customWidth="1"/>
     <col min="8" max="8" width="13.36328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="4">
+        <v>974</v>
+      </c>
+      <c r="D2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" t="s">
         <v>0</v>
       </c>
-      <c r="B2">
-        <v>91</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="F2" s="4">
+        <v>974</v>
+      </c>
+      <c r="G2" t="s">
         <v>1</v>
       </c>
-      <c r="D2" t="s">
+      <c r="H2" t="s">
         <v>2</v>
       </c>
-      <c r="E2" t="s">
-        <v>3</v>
-      </c>
-      <c r="F2">
-        <v>91</v>
-      </c>
-      <c r="G2" t="s">
-        <v>4</v>
-      </c>
-      <c r="H2" t="s">
-        <v>5</v>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added excel upload template
</commit_message>
<xml_diff>
--- a/public/countrystatecity.xlsx
+++ b/public/countrystatecity.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\Stalvin_MM\GulfMall\gulfmall_CMS\public\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lenovo\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A68CE04E-F6BB-4D75-BF96-755C414CE1AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0044FEB4-EC90-4817-85F6-58DDD7C8B411}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,17 +33,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="15">
   <si>
     <t>الهند</t>
   </si>
   <si>
-    <t>كارناتاكا</t>
-  </si>
-  <si>
-    <t>بنغالورو</t>
-  </si>
-  <si>
     <t>Country(en)</t>
   </si>
   <si>
@@ -74,7 +68,16 @@
     <t>Doha</t>
   </si>
   <si>
-    <t>United Arab Emirates</t>
+    <t>الريان</t>
+  </si>
+  <si>
+    <t>Ad Dawhah</t>
+  </si>
+  <si>
+    <t>الدوحة</t>
+  </si>
+  <si>
+    <t>Al Rayyan</t>
   </si>
 </sst>
 </file>
@@ -84,7 +87,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="\+0"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -99,12 +102,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="7"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Courier New"/>
-      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -127,10 +124,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
@@ -440,73 +436,97 @@
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="16.7265625" customWidth="1"/>
-    <col min="2" max="2" width="15" style="4" customWidth="1"/>
+    <col min="2" max="2" width="15" style="3" customWidth="1"/>
     <col min="3" max="3" width="16.453125" customWidth="1"/>
     <col min="4" max="4" width="20.08984375" customWidth="1"/>
     <col min="5" max="5" width="16.453125" customWidth="1"/>
-    <col min="6" max="6" width="15.6328125" style="4" customWidth="1"/>
+    <col min="6" max="6" width="15.6328125" style="3" customWidth="1"/>
     <col min="7" max="7" width="13.08984375" customWidth="1"/>
     <col min="8" max="8" width="13.36328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>4</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" s="4">
+        <v>9</v>
+      </c>
+      <c r="B2" s="3">
         <v>974</v>
       </c>
+      <c r="C2" t="s">
+        <v>12</v>
+      </c>
       <c r="D2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E2" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="4">
+      <c r="F2" s="3">
         <v>974</v>
       </c>
       <c r="G2" t="s">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="H2" t="s">
-        <v>2</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A3" s="2" t="s">
-        <v>13</v>
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="3">
+        <v>974</v>
+      </c>
+      <c r="C3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" t="s">
+        <v>0</v>
+      </c>
+      <c r="F3" s="3">
+        <v>974</v>
+      </c>
+      <c r="G3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H3" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>